<commit_message>
reformating of result computation and saving functions
</commit_message>
<xml_diff>
--- a/msAnalyzer/data/template_not_labeled.xlsx
+++ b/msAnalyzer/data/template_not_labeled.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gui/Git/labUtils/msAnalyzer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{98F4E4FE-4B93-2C4D-AEC5-E9C3AF2D4976}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7F9B36A3-84AB-7D49-9373-AEC5DD56B6C2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7660" yWindow="460" windowWidth="21140" windowHeight="16380" tabRatio="400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1210,7 +1210,7 @@
   <dimension ref="A1:G97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E2" sqref="E2:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>